<commit_message>
Improvements and other tweaks for Win demo
</commit_message>
<xml_diff>
--- a/output/Some_country.xlsx
+++ b/output/Some_country.xlsx
@@ -607,28 +607,28 @@
         <v>5830</v>
       </c>
       <c r="G2" t="n">
-        <v>86.58</v>
+        <v>68.48</v>
       </c>
       <c r="H2" t="n">
-        <v>498.5</v>
+        <v>483.8</v>
       </c>
       <c r="I2" t="n">
-        <v>957.1</v>
+        <v>952.3</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1642</v>
+        <v>0.1633</v>
       </c>
       <c r="K2" t="n">
-        <v>771.5</v>
+        <v>677.2</v>
       </c>
       <c r="L2" t="n">
-        <v>1149</v>
+        <v>1065</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1939</v>
+        <v>0.2888</v>
       </c>
       <c r="N2" t="n">
-        <v>0.201</v>
+        <v>0.1185</v>
       </c>
     </row>
     <row r="3">
@@ -651,28 +651,28 @@
         <v>5910</v>
       </c>
       <c r="G3" t="n">
-        <v>99.24</v>
+        <v>90.03</v>
       </c>
       <c r="H3" t="n">
-        <v>262.2</v>
+        <v>296.6</v>
       </c>
       <c r="I3" t="n">
-        <v>730</v>
+        <v>795.7</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1235</v>
+        <v>0.1346</v>
       </c>
       <c r="K3" t="n">
-        <v>576.5</v>
+        <v>537.8</v>
       </c>
       <c r="L3" t="n">
-        <v>891.7</v>
+        <v>976.7</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2103</v>
+        <v>0.3241</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2215</v>
+        <v>0.2275</v>
       </c>
     </row>
     <row r="4">
@@ -695,28 +695,28 @@
         <v>5830</v>
       </c>
       <c r="G4" t="n">
-        <v>65.9</v>
+        <v>68.48</v>
       </c>
       <c r="H4" t="n">
-        <v>277.1</v>
+        <v>288.1</v>
       </c>
       <c r="I4" t="n">
-        <v>558.5</v>
+        <v>647.7</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09579</v>
+        <v>0.1111</v>
       </c>
       <c r="K4" t="n">
-        <v>415.4</v>
+        <v>392.1</v>
       </c>
       <c r="L4" t="n">
-        <v>670.3</v>
+        <v>791.4</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2562</v>
+        <v>0.3946</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2002</v>
+        <v>0.2219</v>
       </c>
     </row>
   </sheetData>
@@ -899,10 +899,10 @@
         <v>48</v>
       </c>
       <c r="AB2" t="n">
-        <v>22.26</v>
+        <v>17.61</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.2474</v>
+        <v>0.1957</v>
       </c>
     </row>
     <row r="3">
@@ -982,10 +982,10 @@
         <v>48</v>
       </c>
       <c r="AB3" t="n">
-        <v>30.38</v>
+        <v>31.89</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3376</v>
+        <v>0.3543</v>
       </c>
     </row>
     <row r="4">
@@ -1065,10 +1065,10 @@
         <v>48</v>
       </c>
       <c r="AB4" t="n">
-        <v>12.48</v>
+        <v>14.03</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.104</v>
+        <v>0.1169</v>
       </c>
     </row>
     <row r="5">
@@ -1148,10 +1148,10 @@
         <v>58</v>
       </c>
       <c r="AB5" t="n">
-        <v>16.99</v>
+        <v>16.49</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1416</v>
+        <v>0.1374</v>
       </c>
     </row>
     <row r="6">
@@ -1231,10 +1231,10 @@
         <v>48</v>
       </c>
       <c r="AB6" t="n">
-        <v>24.81</v>
+        <v>22.51</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.2363</v>
+        <v>0.2144</v>
       </c>
     </row>
     <row r="7">
@@ -1314,10 +1314,10 @@
         <v>48</v>
       </c>
       <c r="AB7" t="n">
-        <v>26.71</v>
+        <v>31.14</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.2543</v>
+        <v>0.2966</v>
       </c>
     </row>
     <row r="8">
@@ -1397,10 +1397,10 @@
         <v>48</v>
       </c>
       <c r="AB8" t="n">
-        <v>12.96</v>
+        <v>15.52</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.09598</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="9">
@@ -1480,10 +1480,10 @@
         <v>58</v>
       </c>
       <c r="AB9" t="n">
-        <v>9.534</v>
+        <v>9.9</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.07945</v>
+        <v>0.0825</v>
       </c>
     </row>
     <row r="10">
@@ -1563,10 +1563,10 @@
         <v>48</v>
       </c>
       <c r="AB10" t="n">
-        <v>22.26</v>
+        <v>17.61</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.2474</v>
+        <v>0.1957</v>
       </c>
     </row>
     <row r="11">
@@ -1646,10 +1646,10 @@
         <v>48</v>
       </c>
       <c r="AB11" t="n">
-        <v>16.11</v>
+        <v>24.19</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.179</v>
+        <v>0.2688</v>
       </c>
     </row>
     <row r="12">
@@ -1729,10 +1729,10 @@
         <v>48</v>
       </c>
       <c r="AB12" t="n">
-        <v>6.378</v>
+        <v>9.441</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.05315</v>
+        <v>0.07867</v>
       </c>
     </row>
     <row r="13">
@@ -1812,10 +1812,10 @@
         <v>58</v>
       </c>
       <c r="AB13" t="n">
-        <v>9.446</v>
+        <v>9.821</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.07872</v>
+        <v>0.08184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
earlier work, may be incomplete!
</commit_message>
<xml_diff>
--- a/output/Some_country.xlsx
+++ b/output/Some_country.xlsx
@@ -629,22 +629,22 @@
         <v>5830</v>
       </c>
       <c r="G2" t="n">
-        <v>71.79</v>
+        <v>71.01</v>
       </c>
       <c r="H2" t="n">
-        <v>501.5</v>
+        <v>504.6</v>
       </c>
       <c r="I2" t="n">
-        <v>953.7</v>
+        <v>961.4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1636</v>
+        <v>0.1649</v>
       </c>
       <c r="K2" t="n">
-        <v>866.8</v>
+        <v>836.1</v>
       </c>
       <c r="L2" t="n">
-        <v>1224</v>
+        <v>1214</v>
       </c>
       <c r="M2" t="n">
         <v>5216</v>
@@ -653,10 +653,10 @@
         <v>6543</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1503</v>
+        <v>0.1451</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2047</v>
+        <v>0.202</v>
       </c>
     </row>
     <row r="3">
@@ -679,22 +679,22 @@
         <v>5910</v>
       </c>
       <c r="G3" t="n">
-        <v>81.44</v>
+        <v>80.86</v>
       </c>
       <c r="H3" t="n">
-        <v>345.6</v>
+        <v>290.5</v>
       </c>
       <c r="I3" t="n">
-        <v>810</v>
+        <v>758.9</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1371</v>
+        <v>0.1284</v>
       </c>
       <c r="K3" t="n">
-        <v>668.9</v>
+        <v>630.9</v>
       </c>
       <c r="L3" t="n">
-        <v>1040</v>
+        <v>951.3</v>
       </c>
       <c r="M3" t="n">
         <v>5287</v>
@@ -703,10 +703,10 @@
         <v>6632</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1134</v>
+        <v>0.1111</v>
       </c>
       <c r="P3" t="n">
-        <v>0.164</v>
+        <v>0.1552</v>
       </c>
     </row>
     <row r="4">
@@ -729,22 +729,22 @@
         <v>5830</v>
       </c>
       <c r="G4" t="n">
-        <v>71.79</v>
+        <v>71.01</v>
       </c>
       <c r="H4" t="n">
-        <v>369</v>
+        <v>310.2</v>
       </c>
       <c r="I4" t="n">
-        <v>697</v>
+        <v>614.6</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1196</v>
+        <v>0.1054</v>
       </c>
       <c r="K4" t="n">
-        <v>529.4</v>
+        <v>472.5</v>
       </c>
       <c r="L4" t="n">
-        <v>881.2</v>
+        <v>807.3</v>
       </c>
       <c r="M4" t="n">
         <v>5216</v>
@@ -753,10 +753,10 @@
         <v>6543</v>
       </c>
       <c r="O4" t="n">
-        <v>0.09052</v>
+        <v>0.0789</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1406</v>
+        <v>0.1285</v>
       </c>
     </row>
   </sheetData>
@@ -849,22 +849,22 @@
         <v>1070</v>
       </c>
       <c r="H2" t="n">
-        <v>71.79</v>
+        <v>71.01</v>
       </c>
       <c r="I2" t="n">
-        <v>249.9</v>
+        <v>257.1</v>
       </c>
       <c r="J2" t="n">
-        <v>321.7</v>
+        <v>328.1</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3007</v>
+        <v>0.3066</v>
       </c>
       <c r="L2" t="n">
-        <v>223.4</v>
+        <v>208.4</v>
       </c>
       <c r="M2" t="n">
-        <v>417</v>
+        <v>432.9</v>
       </c>
       <c r="N2" t="n">
         <v>957.3</v>
@@ -873,10 +873,10 @@
         <v>1201</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2093</v>
+        <v>0.1942</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.3822</v>
+        <v>0.3882</v>
       </c>
     </row>
     <row r="3">
@@ -902,22 +902,22 @@
         <v>4760</v>
       </c>
       <c r="H3" t="n">
-        <v>130.4</v>
+        <v>128.7</v>
       </c>
       <c r="I3" t="n">
-        <v>501.5</v>
+        <v>504.6</v>
       </c>
       <c r="J3" t="n">
-        <v>632</v>
+        <v>633.3</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1328</v>
+        <v>0.1331</v>
       </c>
       <c r="L3" t="n">
-        <v>592.5</v>
+        <v>543.5</v>
       </c>
       <c r="M3" t="n">
-        <v>867.1</v>
+        <v>862.1</v>
       </c>
       <c r="N3" t="n">
         <v>4258</v>
@@ -926,10 +926,10 @@
         <v>5342</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1253</v>
+        <v>0.1199</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1746</v>
+        <v>0.1799</v>
       </c>
     </row>
     <row r="4">
@@ -955,22 +955,22 @@
         <v>1420</v>
       </c>
       <c r="H4" t="n">
-        <v>81.44</v>
+        <v>80.86</v>
       </c>
       <c r="I4" t="n">
-        <v>260.1</v>
+        <v>266.2</v>
       </c>
       <c r="J4" t="n">
-        <v>341.6</v>
+        <v>347</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2406</v>
+        <v>0.2444</v>
       </c>
       <c r="L4" t="n">
-        <v>258.8</v>
+        <v>254.6</v>
       </c>
       <c r="M4" t="n">
-        <v>457.8</v>
+        <v>466.9</v>
       </c>
       <c r="N4" t="n">
         <v>1270</v>
@@ -979,10 +979,10 @@
         <v>1594</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1761</v>
+        <v>0.1766</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.3133</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="5">
@@ -1008,22 +1008,22 @@
         <v>4490</v>
       </c>
       <c r="H5" t="n">
-        <v>122.8</v>
+        <v>121.3</v>
       </c>
       <c r="I5" t="n">
-        <v>345.6</v>
+        <v>290.5</v>
       </c>
       <c r="J5" t="n">
-        <v>468.5</v>
+        <v>411.9</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1043</v>
+        <v>0.09173</v>
       </c>
       <c r="L5" t="n">
-        <v>367.2</v>
+        <v>317.1</v>
       </c>
       <c r="M5" t="n">
-        <v>599.2</v>
+        <v>553.5</v>
       </c>
       <c r="N5" t="n">
         <v>4017</v>
@@ -1032,10 +1032,10 @@
         <v>5039</v>
       </c>
       <c r="P5" t="n">
-        <v>0.083</v>
+        <v>0.0768</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1259</v>
+        <v>0.1184</v>
       </c>
     </row>
     <row r="6">
@@ -1061,22 +1061,22 @@
         <v>1070</v>
       </c>
       <c r="H6" t="n">
-        <v>71.79</v>
+        <v>71.01</v>
       </c>
       <c r="I6" t="n">
-        <v>141.2</v>
+        <v>139.3</v>
       </c>
       <c r="J6" t="n">
-        <v>213</v>
+        <v>210.3</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1991</v>
+        <v>0.1966</v>
       </c>
       <c r="L6" t="n">
-        <v>174.1</v>
+        <v>162.3</v>
       </c>
       <c r="M6" t="n">
-        <v>253.6</v>
+        <v>246.1</v>
       </c>
       <c r="N6" t="n">
         <v>957.3</v>
@@ -1085,10 +1085,10 @@
         <v>1201</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1576</v>
+        <v>0.149</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.2305</v>
+        <v>0.2174</v>
       </c>
     </row>
     <row r="7">
@@ -1114,22 +1114,22 @@
         <v>4760</v>
       </c>
       <c r="H7" t="n">
-        <v>115</v>
+        <v>94.03</v>
       </c>
       <c r="I7" t="n">
-        <v>369</v>
+        <v>310.2</v>
       </c>
       <c r="J7" t="n">
-        <v>484</v>
+        <v>404.2</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1017</v>
+        <v>0.08492</v>
       </c>
       <c r="L7" t="n">
-        <v>350.3</v>
+        <v>291</v>
       </c>
       <c r="M7" t="n">
-        <v>616.3</v>
+        <v>573.1</v>
       </c>
       <c r="N7" t="n">
         <v>4258</v>
@@ -1138,10 +1138,10 @@
         <v>5342</v>
       </c>
       <c r="P7" t="n">
-        <v>0.07356</v>
+        <v>0.06158</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1253</v>
+        <v>0.1145</v>
       </c>
     </row>
   </sheetData>
@@ -1324,10 +1324,10 @@
         <v>53</v>
       </c>
       <c r="AB2" t="n">
-        <v>18.46</v>
+        <v>18.26</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.2051</v>
+        <v>0.2029</v>
       </c>
     </row>
     <row r="3">
@@ -1407,10 +1407,10 @@
         <v>53</v>
       </c>
       <c r="AB3" t="n">
-        <v>31.24</v>
+        <v>32.14</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3471</v>
+        <v>0.3571</v>
       </c>
     </row>
     <row r="4">
@@ -1490,10 +1490,10 @@
         <v>53</v>
       </c>
       <c r="AB4" t="n">
-        <v>12.62</v>
+        <v>12.46</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.1052</v>
+        <v>0.1038</v>
       </c>
     </row>
     <row r="5">
@@ -1573,10 +1573,10 @@
         <v>63</v>
       </c>
       <c r="AB5" t="n">
-        <v>17.1</v>
+        <v>17.2</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1425</v>
+        <v>0.1434</v>
       </c>
     </row>
     <row r="6">
@@ -1656,10 +1656,10 @@
         <v>53</v>
       </c>
       <c r="AB6" t="n">
-        <v>20.36</v>
+        <v>20.22</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.1939</v>
+        <v>0.1925</v>
       </c>
     </row>
     <row r="7">
@@ -1739,10 +1739,10 @@
         <v>53</v>
       </c>
       <c r="AB7" t="n">
-        <v>27.32</v>
+        <v>27.95</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.2601</v>
+        <v>0.2662</v>
       </c>
     </row>
     <row r="8">
@@ -1822,10 +1822,10 @@
         <v>53</v>
       </c>
       <c r="AB8" t="n">
-        <v>13.94</v>
+        <v>13.77</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1032</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="9">
@@ -1905,10 +1905,10 @@
         <v>63</v>
       </c>
       <c r="AB9" t="n">
-        <v>12.57</v>
+        <v>10.56</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.1047</v>
+        <v>0.08804</v>
       </c>
     </row>
     <row r="10">
@@ -1988,10 +1988,10 @@
         <v>53</v>
       </c>
       <c r="AB10" t="n">
-        <v>18.46</v>
+        <v>18.26</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.2051</v>
+        <v>0.2029</v>
       </c>
     </row>
     <row r="11">
@@ -2071,10 +2071,10 @@
         <v>53</v>
       </c>
       <c r="AB11" t="n">
-        <v>17.65</v>
+        <v>17.42</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1961</v>
+        <v>0.1935</v>
       </c>
     </row>
     <row r="12">
@@ -2154,10 +2154,10 @@
         <v>53</v>
       </c>
       <c r="AB12" t="n">
-        <v>11.13</v>
+        <v>9.1</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.09276</v>
+        <v>0.07583</v>
       </c>
     </row>
     <row r="13">
@@ -2237,10 +2237,10 @@
         <v>63</v>
       </c>
       <c r="AB13" t="n">
-        <v>12.58</v>
+        <v>10.58</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.1048</v>
+        <v>0.08813</v>
       </c>
     </row>
   </sheetData>

</xml_diff>